<commit_message>
Adds table and all stuff
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -150,44 +150,49 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Notes</t>
+          <t>الملاحظات</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>التحكم</t>
         </is>
       </c>
     </row>
     <row r="2" spans="1:13" customHeight="0">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>4442</t>
+          <t>4386</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>363402003959</t>
+          <t>711013002113</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>231024244</t>
+          <t>007960</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>559339612</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>معايير</t>
+          <t>عائن</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>المذنب - قرطبة</t>
+          <t>الرمال</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>عبد العزيز السهلي</t>
         </is>
       </c>
       <c r="J2" s="2" t="inlineStr">
@@ -209,22 +214,22 @@
     <row r="3" spans="1:13" customHeight="0">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>4441</t>
+          <t>4385</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>غير واضح</t>
+          <t>311004005388</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>50823335‏</t>
+          <t>016430</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>563528999</t>
+          <t>563688118</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr">
@@ -234,14 +239,14 @@
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>المجمعة</t>
+          <t>النهضة</t>
         </is>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3" t="inlineStr">
         <is>
-          <t>المتعاون عبد الاله</t>
+          <t>عبد العزيز السهلي</t>
         </is>
       </c>
       <c r="J3" s="3" t="inlineStr">
@@ -251,7 +256,7 @@
       </c>
       <c r="K3" s="3" t="inlineStr">
         <is>
-          <t>&lt;span class='badge badge-pill alert-table badge-danger'&gt;المعاينه&lt;/span&gt;</t>
+          <t>&lt;span class='badge badge-pill alert-table badge-warning'&gt;جديد&lt;/span&gt;</t>
         </is>
       </c>
       <c r="L3" s="3" t="inlineStr">
@@ -260,113 +265,6 @@
         </is>
       </c>
       <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:13" customHeight="0">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>4440</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>31020313190</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>007973</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>530751370</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>عائن</t>
-        </is>
-      </c>
-      <c r="F4" s="2" t="inlineStr">
-        <is>
-          <t>احد - الرياض</t>
-        </is>
-      </c>
-      <c r="I4" s="2" t="inlineStr">
-        <is>
-          <t>احمد السالم</t>
-        </is>
-      </c>
-      <c r="J4" s="2" t="inlineStr">
-        <is>
-          <t>لا</t>
-        </is>
-      </c>
-      <c r="K4" s="2" t="inlineStr">
-        <is>
-          <t>&lt;span class='badge badge-pill alert-table badge-danger'&gt;المعاينه&lt;/span&gt;</t>
-        </is>
-      </c>
-      <c r="L4" s="2" t="inlineStr">
-        <is>
-          <t>03/10/2023</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" spans="1:13" customHeight="0">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>4439</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>811017003256</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="inlineStr">
-        <is>
-          <t>231000059</t>
-        </is>
-      </c>
-      <c r="D5" s="3" t="inlineStr">
-        <is>
-          <t>557961947</t>
-        </is>
-      </c>
-      <c r="E5" s="3" t="inlineStr">
-        <is>
-          <t>دور شيستر</t>
-        </is>
-      </c>
-      <c r="F5" s="3" t="inlineStr">
-        <is>
-          <t>الدار البيضاء - الرياض</t>
-        </is>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3" t="inlineStr">
-        <is>
-          <t>احمد السالم</t>
-        </is>
-      </c>
-      <c r="J5" s="3" t="inlineStr">
-        <is>
-          <t>لا</t>
-        </is>
-      </c>
-      <c r="K5" s="3" t="inlineStr">
-        <is>
-          <t>&lt;span class='badge badge-pill alert-table badge-danger'&gt;المعاينه&lt;/span&gt;</t>
-        </is>
-      </c>
-      <c r="L5" s="3" t="inlineStr">
-        <is>
-          <t>03/10/2023</t>
-        </is>
-      </c>
-      <c r="M5" s="3"/>
     </row>
   </sheetData>
   <legacyDrawing r:id="rId_comments_vml1"/>

</xml_diff>